<commit_message>
chained DMA ok with 3 ADC channels
</commit_message>
<xml_diff>
--- a/Project Prototype/BOM/Bill of Materials-Autobot_project-Final-V1.xlsx
+++ b/Project Prototype/BOM/Bill of Materials-Autobot_project-Final-V1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Comment</t>
   </si>
@@ -282,6 +282,33 @@
   </si>
   <si>
     <t>2527545</t>
+  </si>
+  <si>
+    <t>Recu</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>KP-1608SURCK</t>
+  </si>
+  <si>
+    <t>KP-1608MGC</t>
+  </si>
+  <si>
+    <t>2290329</t>
+  </si>
+  <si>
+    <t>8529825</t>
+  </si>
+  <si>
+    <t>KINGBRIGHT</t>
+  </si>
+  <si>
+    <t>ref issue!</t>
+  </si>
+  <si>
+    <t>won't be ordered</t>
   </si>
 </sst>
 </file>
@@ -317,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -340,17 +367,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +704,7 @@
     <col min="11" max="11" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,8 +738,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -721,8 +776,11 @@
       <c r="K2" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -756,8 +814,11 @@
       <c r="K3" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -791,8 +852,11 @@
       <c r="K4" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -812,22 +876,25 @@
         <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -847,22 +914,25 @@
         <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M6" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -896,8 +966,11 @@
       <c r="K7" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -931,8 +1004,11 @@
       <c r="K8" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -966,8 +1042,11 @@
       <c r="K9" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>55</v>
       </c>
@@ -1001,8 +1080,11 @@
       <c r="K10" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
@@ -1036,8 +1118,11 @@
       <c r="K11" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -1071,8 +1156,11 @@
       <c r="K12" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
@@ -1106,8 +1194,11 @@
       <c r="K13" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>65</v>
       </c>
@@ -1142,7 +1233,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -1173,6 +1264,9 @@
       </c>
       <c r="K15" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>